<commit_message>
Add generated leaderboard data - 2024-03-12T19:48:58
</commit_message>
<xml_diff>
--- a/Leaderboards/CurrentCMRITLeaderboard2025.xlsx
+++ b/Leaderboards/CurrentCMRITLeaderboard2025.xlsx
@@ -13440,7 +13440,7 @@
         <v>21</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>789.0</v>
+        <v>817.0</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>22</v>
@@ -13572,7 +13572,7 @@
         <v>35</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>664.0</v>
+        <v>629.0</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>36</v>
@@ -13681,7 +13681,7 @@
         <v>43</v>
       </c>
       <c r="K8" s="2" t="n">
-        <v>1312.0</v>
+        <v>979.0</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>44</v>
@@ -13748,7 +13748,7 @@
         <v>50</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>831.0</v>
+        <v>774.0</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>51</v>
@@ -14056,7 +14056,7 @@
         <v>74</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>545.0</v>
+        <v>611.0</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>75</v>
@@ -14408,7 +14408,7 @@
         <v>108</v>
       </c>
       <c r="D25" s="2" t="n">
-        <v>678.0</v>
+        <v>841.0</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>109</v>
@@ -15156,7 +15156,7 @@
         <v>178</v>
       </c>
       <c r="D42" s="2" t="n">
-        <v>355.0</v>
+        <v>589.0</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>179</v>
@@ -15288,7 +15288,7 @@
         <v>192</v>
       </c>
       <c r="D45" s="2" t="n">
-        <v>750.0</v>
+        <v>707.0</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>193</v>
@@ -15749,7 +15749,7 @@
         <v>235</v>
       </c>
       <c r="K55" s="2" t="n">
-        <v>1445.0</v>
+        <v>1128.0</v>
       </c>
       <c r="L55" s="2" t="s">
         <v>233</v>
@@ -16168,7 +16168,7 @@
         <v>276</v>
       </c>
       <c r="D65" s="2" t="n">
-        <v>567.0</v>
+        <v>693.0</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>277</v>
@@ -16432,7 +16432,7 @@
         <v>294</v>
       </c>
       <c r="D71" s="2" t="n">
-        <v>644.0</v>
+        <v>763.0</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>27</v>
@@ -16564,7 +16564,7 @@
         <v>309</v>
       </c>
       <c r="D74" s="2" t="n">
-        <v>822.0</v>
+        <v>844.0</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>310</v>
@@ -16828,7 +16828,7 @@
         <v>335</v>
       </c>
       <c r="D80" s="2" t="n">
-        <v>354.0</v>
+        <v>619.0</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>336</v>
@@ -17224,7 +17224,7 @@
         <v>365</v>
       </c>
       <c r="D89" s="2" t="n">
-        <v>893.0</v>
+        <v>1026.0</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>366</v>
@@ -17245,7 +17245,7 @@
         <v>368</v>
       </c>
       <c r="K89" s="2" t="n">
-        <v>1092.0</v>
+        <v>764.0</v>
       </c>
       <c r="L89" s="2" t="s">
         <v>367</v>
@@ -17664,7 +17664,7 @@
         <v>406</v>
       </c>
       <c r="D99" s="2" t="n">
-        <v>778.0</v>
+        <v>791.0</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>407</v>
@@ -18104,7 +18104,7 @@
         <v>450</v>
       </c>
       <c r="D109" s="2" t="n">
-        <v>865.0</v>
+        <v>759.0</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>450</v>
@@ -18984,7 +18984,7 @@
         <v>527</v>
       </c>
       <c r="D129" s="2" t="n">
-        <v>703.0</v>
+        <v>898.0</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>527</v>
@@ -20128,7 +20128,7 @@
         <v>622</v>
       </c>
       <c r="D155" s="2" t="n">
-        <v>743.0</v>
+        <v>643.0</v>
       </c>
       <c r="E155" s="2" t="s">
         <v>623</v>
@@ -20260,7 +20260,7 @@
         <v>636</v>
       </c>
       <c r="D158" s="2" t="n">
-        <v>601.0</v>
+        <v>826.0</v>
       </c>
       <c r="E158" s="2" t="s">
         <v>637</v>
@@ -20832,7 +20832,7 @@
         <v>692</v>
       </c>
       <c r="D171" s="2" t="n">
-        <v>0.0</v>
+        <v>357.0</v>
       </c>
       <c r="E171" s="2" t="s">
         <v>693</v>
@@ -21492,7 +21492,7 @@
         <v>765</v>
       </c>
       <c r="D186" s="2" t="n">
-        <v>748.0</v>
+        <v>742.0</v>
       </c>
       <c r="E186" s="2" t="s">
         <v>766</v>
@@ -21580,7 +21580,7 @@
         <v>773</v>
       </c>
       <c r="D188" s="2" t="n">
-        <v>0.0</v>
+        <v>381.0</v>
       </c>
       <c r="E188" s="2" t="s">
         <v>773</v>
@@ -21624,7 +21624,7 @@
         <v>777</v>
       </c>
       <c r="D189" s="2" t="n">
-        <v>897.0</v>
+        <v>1007.0</v>
       </c>
       <c r="E189" s="2" t="s">
         <v>778</v>
@@ -22328,7 +22328,7 @@
         <v>837</v>
       </c>
       <c r="D205" s="2" t="n">
-        <v>0.0</v>
+        <v>360.0</v>
       </c>
       <c r="E205" s="2" t="s">
         <v>838</v>
@@ -23560,7 +23560,7 @@
         <v>933</v>
       </c>
       <c r="D233" s="2" t="n">
-        <v>848.0</v>
+        <v>847.0</v>
       </c>
       <c r="E233" s="2" t="s">
         <v>934</v>
@@ -23736,7 +23736,7 @@
         <v>952</v>
       </c>
       <c r="D237" s="2" t="n">
-        <v>836.0</v>
+        <v>865.0</v>
       </c>
       <c r="E237" s="2" t="s">
         <v>953</v>
@@ -24616,7 +24616,7 @@
         <v>1027</v>
       </c>
       <c r="D257" s="2" t="n">
-        <v>854.0</v>
+        <v>842.0</v>
       </c>
       <c r="E257" s="2" t="s">
         <v>1028</v>
@@ -24880,7 +24880,7 @@
         <v>1046</v>
       </c>
       <c r="D263" s="2" t="n">
-        <v>659.0</v>
+        <v>563.0</v>
       </c>
       <c r="E263" s="2" t="s">
         <v>1047</v>
@@ -25276,7 +25276,7 @@
         <v>1069</v>
       </c>
       <c r="D272" s="2" t="n">
-        <v>773.0</v>
+        <v>829.0</v>
       </c>
       <c r="E272" s="2" t="s">
         <v>1070</v>
@@ -25452,7 +25452,7 @@
         <v>1088</v>
       </c>
       <c r="D276" s="2" t="n">
-        <v>890.0</v>
+        <v>901.0</v>
       </c>
       <c r="E276" s="2" t="s">
         <v>1089</v>
@@ -25496,7 +25496,7 @@
         <v>1094</v>
       </c>
       <c r="D277" s="2" t="n">
-        <v>651.0</v>
+        <v>795.0</v>
       </c>
       <c r="E277" s="2" t="s">
         <v>1095</v>
@@ -25672,7 +25672,7 @@
         <v>1116</v>
       </c>
       <c r="D281" s="2" t="n">
-        <v>773.0</v>
+        <v>715.0</v>
       </c>
       <c r="E281" s="2" t="s">
         <v>1117</v>
@@ -26353,7 +26353,7 @@
         <v>1178</v>
       </c>
       <c r="K296" s="2" t="n">
-        <v>1155.0</v>
+        <v>821.0</v>
       </c>
       <c r="L296" s="2" t="s">
         <v>1180</v>
@@ -26772,7 +26772,7 @@
         <v>1217</v>
       </c>
       <c r="D306" s="2" t="n">
-        <v>752.0</v>
+        <v>740.0</v>
       </c>
       <c r="E306" s="2" t="s">
         <v>1218</v>
@@ -26860,7 +26860,7 @@
         <v>1226</v>
       </c>
       <c r="D308" s="2" t="n">
-        <v>696.0</v>
+        <v>730.0</v>
       </c>
       <c r="E308" s="2" t="s">
         <v>1227</v>
@@ -26904,7 +26904,7 @@
         <v>1230</v>
       </c>
       <c r="D309" s="2" t="n">
-        <v>732.0</v>
+        <v>791.0</v>
       </c>
       <c r="E309" s="2" t="s">
         <v>1231</v>
@@ -27080,7 +27080,7 @@
         <v>1245</v>
       </c>
       <c r="D313" s="2" t="n">
-        <v>860.0</v>
+        <v>913.0</v>
       </c>
       <c r="E313" s="2" t="s">
         <v>1246</v>
@@ -27256,7 +27256,7 @@
         <v>1260</v>
       </c>
       <c r="D317" s="2" t="n">
-        <v>558.0</v>
+        <v>533.0</v>
       </c>
       <c r="E317" s="2" t="s">
         <v>1261</v>
@@ -27300,7 +27300,7 @@
         <v>1266</v>
       </c>
       <c r="D318" s="2" t="n">
-        <v>737.0</v>
+        <v>769.0</v>
       </c>
       <c r="E318" s="2" t="s">
         <v>1267</v>
@@ -27872,7 +27872,7 @@
         <v>1315</v>
       </c>
       <c r="D331" s="2" t="n">
-        <v>701.0</v>
+        <v>753.0</v>
       </c>
       <c r="E331" s="2" t="s">
         <v>1316</v>
@@ -28004,7 +28004,7 @@
         <v>1325</v>
       </c>
       <c r="D334" s="2" t="n">
-        <v>749.0</v>
+        <v>913.0</v>
       </c>
       <c r="E334" s="2" t="s">
         <v>1326</v>
@@ -28025,7 +28025,7 @@
         <v>1328</v>
       </c>
       <c r="K334" s="2" t="n">
-        <v>876.0</v>
+        <v>438.0</v>
       </c>
       <c r="L334" s="2" t="s">
         <v>1327</v>
@@ -28092,7 +28092,7 @@
         <v>1334</v>
       </c>
       <c r="D336" s="2" t="n">
-        <v>1166.0</v>
+        <v>1222.0</v>
       </c>
       <c r="E336" s="2" t="s">
         <v>1335</v>
@@ -28356,7 +28356,7 @@
         <v>1356</v>
       </c>
       <c r="D342" s="2" t="n">
-        <v>670.0</v>
+        <v>732.0</v>
       </c>
       <c r="E342" s="2" t="s">
         <v>1357</v>
@@ -28444,7 +28444,7 @@
         <v>1366</v>
       </c>
       <c r="D344" s="2" t="n">
-        <v>813.0</v>
+        <v>845.0</v>
       </c>
       <c r="E344" s="2" t="s">
         <v>1367</v>
@@ -28509,7 +28509,7 @@
         <v>1375</v>
       </c>
       <c r="K345" s="2" t="n">
-        <v>1328.0</v>
+        <v>962.0</v>
       </c>
       <c r="L345" s="2" t="s">
         <v>1374</v>
@@ -28708,7 +28708,7 @@
         <v>1391</v>
       </c>
       <c r="D350" s="2" t="n">
-        <v>791.0</v>
+        <v>781.0</v>
       </c>
       <c r="E350" s="2" t="s">
         <v>1392</v>
@@ -28796,7 +28796,7 @@
         <v>1400</v>
       </c>
       <c r="D352" s="2" t="n">
-        <v>348.0</v>
+        <v>563.0</v>
       </c>
       <c r="E352" s="2" t="s">
         <v>1401</v>
@@ -29500,7 +29500,7 @@
         <v>1460</v>
       </c>
       <c r="D368" s="2" t="n">
-        <v>578.0</v>
+        <v>717.0</v>
       </c>
       <c r="E368" s="2" t="s">
         <v>1461</v>
@@ -29521,7 +29521,7 @@
         <v>1463</v>
       </c>
       <c r="K368" s="2" t="n">
-        <v>1237.0</v>
+        <v>904.0</v>
       </c>
       <c r="L368" s="2" t="s">
         <v>1462</v>
@@ -29741,7 +29741,7 @@
         <v>1484</v>
       </c>
       <c r="K373" s="2" t="n">
-        <v>1393.0</v>
+        <v>1066.0</v>
       </c>
       <c r="L373" s="2" t="s">
         <v>1485</v>
@@ -29785,7 +29785,7 @@
         <v>1489</v>
       </c>
       <c r="K374" s="2" t="n">
-        <v>1418.0</v>
+        <v>1090.0</v>
       </c>
       <c r="L374" s="2" t="s">
         <v>1490</v>
@@ -29808,7 +29808,7 @@
         <v>1492</v>
       </c>
       <c r="D375" s="2" t="n">
-        <v>791.0</v>
+        <v>783.0</v>
       </c>
       <c r="E375" s="2" t="s">
         <v>1493</v>
@@ -30116,7 +30116,7 @@
         <v>1528</v>
       </c>
       <c r="D382" s="2" t="n">
-        <v>352.0</v>
+        <v>572.0</v>
       </c>
       <c r="E382" s="2" t="s">
         <v>1528</v>
@@ -30424,7 +30424,7 @@
         <v>1554</v>
       </c>
       <c r="D389" s="2" t="n">
-        <v>770.0</v>
+        <v>781.0</v>
       </c>
       <c r="E389" s="2" t="s">
         <v>1555</v>
@@ -30468,7 +30468,7 @@
         <v>1560</v>
       </c>
       <c r="D390" s="2" t="n">
-        <v>768.0</v>
+        <v>773.0</v>
       </c>
       <c r="E390" s="2" t="s">
         <v>1561</v>
@@ -30512,7 +30512,7 @@
         <v>1566</v>
       </c>
       <c r="D391" s="2" t="n">
-        <v>556.0</v>
+        <v>644.0</v>
       </c>
       <c r="E391" s="2" t="s">
         <v>1566</v>
@@ -31128,7 +31128,7 @@
         <v>1620</v>
       </c>
       <c r="D405" s="2" t="n">
-        <v>661.0</v>
+        <v>599.0</v>
       </c>
       <c r="E405" s="2" t="s">
         <v>1621</v>
@@ -31172,7 +31172,7 @@
         <v>1624</v>
       </c>
       <c r="D406" s="2" t="n">
-        <v>799.0</v>
+        <v>789.0</v>
       </c>
       <c r="E406" s="2" t="s">
         <v>1625</v>
@@ -31568,7 +31568,7 @@
         <v>1669</v>
       </c>
       <c r="D415" s="2" t="n">
-        <v>754.0</v>
+        <v>863.0</v>
       </c>
       <c r="E415" s="2" t="s">
         <v>1670</v>
@@ -31589,7 +31589,7 @@
         <v>1672</v>
       </c>
       <c r="K415" s="2" t="n">
-        <v>927.0</v>
+        <v>573.0</v>
       </c>
       <c r="L415" s="2" t="s">
         <v>1673</v>
@@ -31744,7 +31744,7 @@
         <v>1687</v>
       </c>
       <c r="D419" s="2" t="n">
-        <v>927.0</v>
+        <v>952.0</v>
       </c>
       <c r="E419" s="2" t="s">
         <v>1688</v>
@@ -31985,7 +31985,7 @@
         <v>1711</v>
       </c>
       <c r="K424" s="2" t="n">
-        <v>1006.0</v>
+        <v>681.0</v>
       </c>
       <c r="L424" s="2" t="s">
         <v>1709</v>
@@ -32184,7 +32184,7 @@
         <v>1724</v>
       </c>
       <c r="D429" s="2" t="n">
-        <v>742.0</v>
+        <v>837.0</v>
       </c>
       <c r="E429" s="2" t="s">
         <v>1724</v>
@@ -32272,7 +32272,7 @@
         <v>1731</v>
       </c>
       <c r="D431" s="2" t="n">
-        <v>628.0</v>
+        <v>613.0</v>
       </c>
       <c r="E431" s="2" t="s">
         <v>1732</v>
@@ -32668,7 +32668,7 @@
         <v>1763</v>
       </c>
       <c r="D440" s="2" t="n">
-        <v>734.0</v>
+        <v>780.0</v>
       </c>
       <c r="E440" s="2" t="s">
         <v>1764</v>
@@ -32756,7 +32756,7 @@
         <v>1771</v>
       </c>
       <c r="D442" s="2" t="n">
-        <v>689.0</v>
+        <v>673.0</v>
       </c>
       <c r="E442" s="2" t="s">
         <v>1772</v>
@@ -33372,7 +33372,7 @@
         <v>1826</v>
       </c>
       <c r="D456" s="2" t="n">
-        <v>686.0</v>
+        <v>640.0</v>
       </c>
       <c r="E456" s="2" t="s">
         <v>1826</v>
@@ -33504,7 +33504,7 @@
         <v>1840</v>
       </c>
       <c r="D459" s="2" t="n">
-        <v>849.0</v>
+        <v>834.0</v>
       </c>
       <c r="E459" s="2" t="s">
         <v>1841</v>
@@ -33636,7 +33636,7 @@
         <v>1854</v>
       </c>
       <c r="D462" s="2" t="n">
-        <v>757.0</v>
+        <v>831.0</v>
       </c>
       <c r="E462" s="2" t="s">
         <v>1855</v>
@@ -34428,7 +34428,7 @@
         <v>1924</v>
       </c>
       <c r="D480" s="2" t="n">
-        <v>750.0</v>
+        <v>781.0</v>
       </c>
       <c r="E480" s="2" t="s">
         <v>1925</v>
@@ -34560,7 +34560,7 @@
         <v>1940</v>
       </c>
       <c r="D483" s="2" t="n">
-        <v>835.0</v>
+        <v>731.0</v>
       </c>
       <c r="E483" s="2" t="s">
         <v>1940</v>
@@ -34604,7 +34604,7 @@
         <v>1943</v>
       </c>
       <c r="D484" s="2" t="n">
-        <v>894.0</v>
+        <v>930.0</v>
       </c>
       <c r="E484" s="2" t="s">
         <v>1944</v>
@@ -34736,7 +34736,7 @@
         <v>1952</v>
       </c>
       <c r="D487" s="2" t="n">
-        <v>981.0</v>
+        <v>956.0</v>
       </c>
       <c r="E487" s="2" t="s">
         <v>1952</v>
@@ -35352,7 +35352,7 @@
         <v>2006</v>
       </c>
       <c r="D501" s="2" t="n">
-        <v>578.0</v>
+        <v>761.0</v>
       </c>
       <c r="E501" s="2" t="s">
         <v>2007</v>
@@ -35748,7 +35748,7 @@
         <v>2045</v>
       </c>
       <c r="D510" s="2" t="n">
-        <v>783.0</v>
+        <v>726.0</v>
       </c>
       <c r="E510" s="2" t="s">
         <v>2046</v>
@@ -35836,7 +35836,7 @@
         <v>2054</v>
       </c>
       <c r="D512" s="2" t="n">
-        <v>784.0</v>
+        <v>709.0</v>
       </c>
       <c r="E512" s="2" t="s">
         <v>2055</v>
@@ -35968,7 +35968,7 @@
         <v>2069</v>
       </c>
       <c r="D515" s="2" t="n">
-        <v>852.0</v>
+        <v>790.0</v>
       </c>
       <c r="E515" s="2" t="s">
         <v>2070</v>
@@ -36012,7 +36012,7 @@
         <v>2073</v>
       </c>
       <c r="D516" s="2" t="n">
-        <v>533.0</v>
+        <v>563.0</v>
       </c>
       <c r="E516" s="2" t="s">
         <v>2074</v>
@@ -36320,7 +36320,7 @@
         <v>2091</v>
       </c>
       <c r="D523" s="2" t="n">
-        <v>814.0</v>
+        <v>734.0</v>
       </c>
       <c r="E523" s="2" t="s">
         <v>2092</v>
@@ -36364,7 +36364,7 @@
         <v>2095</v>
       </c>
       <c r="D524" s="2" t="n">
-        <v>860.0</v>
+        <v>777.0</v>
       </c>
       <c r="E524" s="2" t="s">
         <v>2096</v>
@@ -36760,7 +36760,7 @@
         <v>2131</v>
       </c>
       <c r="D533" s="2" t="n">
-        <v>494.0</v>
+        <v>563.0</v>
       </c>
       <c r="E533" s="2" t="s">
         <v>2132</v>
@@ -37200,7 +37200,7 @@
         <v>2178</v>
       </c>
       <c r="D543" s="2" t="n">
-        <v>577.0</v>
+        <v>777.0</v>
       </c>
       <c r="E543" s="2" t="s">
         <v>2179</v>
@@ -37948,7 +37948,7 @@
         <v>2242</v>
       </c>
       <c r="D560" s="2" t="n">
-        <v>658.0</v>
+        <v>626.0</v>
       </c>
       <c r="E560" s="2" t="s">
         <v>2243</v>
@@ -37969,7 +37969,7 @@
         <v>2245</v>
       </c>
       <c r="K560" s="2" t="n">
-        <v>1350.0</v>
+        <v>1028.0</v>
       </c>
       <c r="L560" s="2" t="s">
         <v>2243</v>
@@ -38564,7 +38564,7 @@
         <v>2289</v>
       </c>
       <c r="D574" s="2" t="n">
-        <v>982.0</v>
+        <v>894.0</v>
       </c>
       <c r="E574" s="2" t="s">
         <v>2290</v>
@@ -38696,7 +38696,7 @@
         <v>2301</v>
       </c>
       <c r="D577" s="2" t="n">
-        <v>745.0</v>
+        <v>673.0</v>
       </c>
       <c r="E577" s="2" t="s">
         <v>2302</v>
@@ -38740,7 +38740,7 @@
         <v>2305</v>
       </c>
       <c r="D578" s="2" t="n">
-        <v>671.0</v>
+        <v>702.0</v>
       </c>
       <c r="E578" s="2" t="s">
         <v>2306</v>
@@ -38805,7 +38805,7 @@
         <v>2312</v>
       </c>
       <c r="K579" s="2" t="n">
-        <v>563.0</v>
+        <v>172.0</v>
       </c>
       <c r="L579" s="2" t="s">
         <v>2311</v>
@@ -38960,7 +38960,7 @@
         <v>2320</v>
       </c>
       <c r="D583" s="2" t="n">
-        <v>768.0</v>
+        <v>752.0</v>
       </c>
       <c r="E583" s="2" t="s">
         <v>2321</v>
@@ -39708,7 +39708,7 @@
         <v>2378</v>
       </c>
       <c r="D600" s="2" t="n">
-        <v>778.0</v>
+        <v>834.0</v>
       </c>
       <c r="E600" s="2" t="s">
         <v>2379</v>
@@ -39840,7 +39840,7 @@
         <v>2394</v>
       </c>
       <c r="D603" s="2" t="n">
-        <v>694.0</v>
+        <v>785.0</v>
       </c>
       <c r="E603" s="2" t="s">
         <v>2395</v>
@@ -40192,7 +40192,7 @@
         <v>2418</v>
       </c>
       <c r="D611" s="2" t="n">
-        <v>840.0</v>
+        <v>915.0</v>
       </c>
       <c r="E611" s="2" t="s">
         <v>2419</v>
@@ -40873,7 +40873,7 @@
         <v>2481</v>
       </c>
       <c r="K626" s="2" t="n">
-        <v>1522.0</v>
+        <v>1223.0</v>
       </c>
       <c r="L626" s="2" t="s">
         <v>2480</v>
@@ -40984,7 +40984,7 @@
         <v>2492</v>
       </c>
       <c r="D629" s="2" t="n">
-        <v>628.0</v>
+        <v>764.0</v>
       </c>
       <c r="E629" s="2" t="s">
         <v>2493</v>
@@ -41512,7 +41512,7 @@
         <v>2537</v>
       </c>
       <c r="D641" s="2" t="n">
-        <v>1157.0</v>
+        <v>1207.0</v>
       </c>
       <c r="E641" s="2" t="s">
         <v>2538</v>
@@ -41533,7 +41533,7 @@
         <v>2540</v>
       </c>
       <c r="K641" s="2" t="n">
-        <v>945.0</v>
+        <v>542.0</v>
       </c>
       <c r="L641" s="2" t="s">
         <v>2538</v>
@@ -41732,7 +41732,7 @@
         <v>2562</v>
       </c>
       <c r="D646" s="2" t="n">
-        <v>785.0</v>
+        <v>813.0</v>
       </c>
       <c r="E646" s="2" t="s">
         <v>2563</v>
@@ -42568,7 +42568,7 @@
         <v>2633</v>
       </c>
       <c r="D665" s="2" t="n">
-        <v>844.0</v>
+        <v>865.0</v>
       </c>
       <c r="E665" s="2" t="s">
         <v>2633</v>
@@ -43029,7 +43029,7 @@
         <v>2667</v>
       </c>
       <c r="K675" s="2" t="n">
-        <v>1409.0</v>
+        <v>1059.0</v>
       </c>
       <c r="L675" s="2" t="s">
         <v>2668</v>
@@ -43492,7 +43492,7 @@
         <v>2718</v>
       </c>
       <c r="D686" s="2" t="n">
-        <v>921.0</v>
+        <v>857.0</v>
       </c>
       <c r="E686" s="2" t="s">
         <v>2719</v>
@@ -45405,7 +45405,7 @@
         <v>2889</v>
       </c>
       <c r="K729" s="2" t="n">
-        <v>1421.0</v>
+        <v>1095.0</v>
       </c>
       <c r="L729" s="2" t="s">
         <v>2887</v>
@@ -45648,7 +45648,7 @@
         <v>2909</v>
       </c>
       <c r="D735" s="2" t="n">
-        <v>637.0</v>
+        <v>813.0</v>
       </c>
       <c r="E735" s="2" t="s">
         <v>2910</v>
@@ -47100,7 +47100,7 @@
         <v>3021</v>
       </c>
       <c r="D768" s="2" t="n">
-        <v>611.0</v>
+        <v>599.0</v>
       </c>
       <c r="E768" s="2" t="s">
         <v>3022</v>
@@ -48772,7 +48772,7 @@
         <v>3194</v>
       </c>
       <c r="D806" s="2" t="n">
-        <v>632.0</v>
+        <v>719.0</v>
       </c>
       <c r="E806" s="2" t="s">
         <v>3195</v>
@@ -49080,7 +49080,7 @@
         <v>3226</v>
       </c>
       <c r="D813" s="2" t="n">
-        <v>664.0</v>
+        <v>625.0</v>
       </c>
       <c r="E813" s="2" t="s">
         <v>27</v>
@@ -49872,7 +49872,7 @@
         <v>3285</v>
       </c>
       <c r="D831" s="2" t="n">
-        <v>612.0</v>
+        <v>621.0</v>
       </c>
       <c r="E831" s="2" t="s">
         <v>3286</v>
@@ -50620,7 +50620,7 @@
         <v>3350</v>
       </c>
       <c r="D848" s="2" t="n">
-        <v>931.0</v>
+        <v>1010.0</v>
       </c>
       <c r="E848" s="2" t="s">
         <v>3351</v>
@@ -50905,7 +50905,7 @@
         <v>3370</v>
       </c>
       <c r="K854" s="2" t="n">
-        <v>988.0</v>
+        <v>663.0</v>
       </c>
       <c r="L854" s="2" t="s">
         <v>3371</v>
@@ -52072,7 +52072,7 @@
         <v>3467</v>
       </c>
       <c r="D881" s="2" t="n">
-        <v>724.0</v>
+        <v>764.0</v>
       </c>
       <c r="E881" s="2" t="s">
         <v>3468</v>
@@ -52424,7 +52424,7 @@
         <v>3494</v>
       </c>
       <c r="D889" s="2" t="n">
-        <v>1173.0</v>
+        <v>1243.0</v>
       </c>
       <c r="E889" s="2" t="s">
         <v>3495</v>
@@ -52600,7 +52600,7 @@
         <v>3506</v>
       </c>
       <c r="D893" s="2" t="n">
-        <v>761.0</v>
+        <v>866.0</v>
       </c>
       <c r="E893" s="2" t="s">
         <v>3507</v>
@@ -52820,7 +52820,7 @@
         <v>3525</v>
       </c>
       <c r="D898" s="2" t="n">
-        <v>727.0</v>
+        <v>877.0</v>
       </c>
       <c r="E898" s="2" t="s">
         <v>3526</v>
@@ -53128,7 +53128,7 @@
         <v>3556</v>
       </c>
       <c r="D905" s="2" t="n">
-        <v>770.0</v>
+        <v>707.0</v>
       </c>
       <c r="E905" s="2" t="s">
         <v>3557</v>
@@ -53304,7 +53304,7 @@
         <v>3577</v>
       </c>
       <c r="D909" s="2" t="n">
-        <v>573.0</v>
+        <v>699.0</v>
       </c>
       <c r="E909" s="2" t="s">
         <v>3578</v>
@@ -54404,7 +54404,7 @@
         <v>3679</v>
       </c>
       <c r="D934" s="2" t="n">
-        <v>523.0</v>
+        <v>571.0</v>
       </c>
       <c r="E934" s="2" t="s">
         <v>3680</v>
@@ -55085,7 +55085,7 @@
         <v>3742</v>
       </c>
       <c r="K949" s="2" t="n">
-        <v>932.0</v>
+        <v>538.0</v>
       </c>
       <c r="L949" s="2" t="s">
         <v>3743</v>
@@ -55965,7 +55965,7 @@
         <v>3799</v>
       </c>
       <c r="K969" s="2" t="n">
-        <v>898.0</v>
+        <v>508.0</v>
       </c>
       <c r="L969" s="2" t="s">
         <v>3798</v>
@@ -56384,7 +56384,7 @@
         <v>3822</v>
       </c>
       <c r="D979" s="2" t="n">
-        <v>1171.0</v>
+        <v>1206.0</v>
       </c>
       <c r="E979" s="2" t="s">
         <v>3823</v>
@@ -56560,7 +56560,7 @@
         <v>3831</v>
       </c>
       <c r="D983" s="2" t="n">
-        <v>770.0</v>
+        <v>713.0</v>
       </c>
       <c r="E983" s="2" t="s">
         <v>3831</v>
@@ -57373,7 +57373,7 @@
         <v>3898</v>
       </c>
       <c r="K1001" s="2" t="n">
-        <v>1200.0</v>
+        <v>915.0</v>
       </c>
       <c r="L1001" s="2" t="s">
         <v>3896</v>
@@ -58320,7 +58320,7 @@
         <v>3957</v>
       </c>
       <c r="D1023" s="2" t="n">
-        <v>691.0</v>
+        <v>727.0</v>
       </c>
       <c r="E1023" s="2" t="s">
         <v>3958</v>
@@ -58473,7 +58473,7 @@
         <v>3966</v>
       </c>
       <c r="K1026" s="2" t="n">
-        <v>1044.0</v>
+        <v>758.0</v>
       </c>
       <c r="L1026" s="2" t="s">
         <v>3965</v>
@@ -59156,7 +59156,7 @@
         <v>4022</v>
       </c>
       <c r="D1042" s="2" t="n">
-        <v>939.0</v>
+        <v>917.0</v>
       </c>
       <c r="E1042" s="2" t="s">
         <v>4023</v>
@@ -59705,7 +59705,7 @@
         <v>4068</v>
       </c>
       <c r="K1054" s="2" t="n">
-        <v>1071.0</v>
+        <v>781.0</v>
       </c>
       <c r="L1054" s="2" t="s">
         <v>4069</v>
@@ -60256,7 +60256,7 @@
         <v>4116</v>
       </c>
       <c r="D1067" s="2" t="n">
-        <v>919.0</v>
+        <v>1020.0</v>
       </c>
       <c r="E1067" s="2" t="s">
         <v>4117</v>
@@ -60344,7 +60344,7 @@
         <v>4125</v>
       </c>
       <c r="D1069" s="2" t="n">
-        <v>829.0</v>
+        <v>886.0</v>
       </c>
       <c r="E1069" s="2" t="s">
         <v>4125</v>
@@ -60476,7 +60476,7 @@
         <v>4140</v>
       </c>
       <c r="D1072" s="2" t="n">
-        <v>732.0</v>
+        <v>689.0</v>
       </c>
       <c r="E1072" s="2" t="s">
         <v>4141</v>
@@ -61136,7 +61136,7 @@
         <v>4195</v>
       </c>
       <c r="D1087" s="2" t="n">
-        <v>849.0</v>
+        <v>813.0</v>
       </c>
       <c r="E1087" s="2" t="s">
         <v>4196</v>
@@ -61576,7 +61576,7 @@
         <v>4238</v>
       </c>
       <c r="D1097" s="2" t="n">
-        <v>1031.0</v>
+        <v>1082.0</v>
       </c>
       <c r="E1097" s="2" t="s">
         <v>4239</v>
@@ -61620,7 +61620,7 @@
         <v>4244</v>
       </c>
       <c r="D1098" s="2" t="n">
-        <v>820.0</v>
+        <v>880.0</v>
       </c>
       <c r="E1098" s="2" t="s">
         <v>4245</v>
@@ -61884,7 +61884,7 @@
         <v>4273</v>
       </c>
       <c r="D1104" s="2" t="n">
-        <v>870.0</v>
+        <v>882.0</v>
       </c>
       <c r="E1104" s="2" t="s">
         <v>4274</v>
@@ -61972,7 +61972,7 @@
         <v>4285</v>
       </c>
       <c r="D1106" s="2" t="n">
-        <v>593.0</v>
+        <v>617.0</v>
       </c>
       <c r="E1106" s="2" t="s">
         <v>4286</v>
@@ -62104,7 +62104,7 @@
         <v>4301</v>
       </c>
       <c r="D1109" s="2" t="n">
-        <v>732.0</v>
+        <v>687.0</v>
       </c>
       <c r="E1109" s="2" t="s">
         <v>4302</v>
@@ -62236,7 +62236,7 @@
         <v>4313</v>
       </c>
       <c r="D1112" s="2" t="n">
-        <v>967.0</v>
+        <v>1082.0</v>
       </c>
       <c r="E1112" s="2" t="s">
         <v>4313</v>
@@ -62852,7 +62852,7 @@
         <v>4371</v>
       </c>
       <c r="D1126" s="2" t="n">
-        <v>670.0</v>
+        <v>640.0</v>
       </c>
       <c r="E1126" s="2" t="s">
         <v>4372</v>
@@ -63116,7 +63116,7 @@
         <v>4397</v>
       </c>
       <c r="D1132" s="2" t="n">
-        <v>702.0</v>
+        <v>817.0</v>
       </c>
       <c r="E1132" s="2" t="s">
         <v>4398</v>

</xml_diff>